<commit_message>
fixed a parallel run failure due to some login test data comes from the excelsheet
</commit_message>
<xml_diff>
--- a/data_sheets/user_credentials.xlsx
+++ b/data_sheets/user_credentials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="valid_logins" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -30,21 +30,6 @@
   </si>
   <si>
     <t>ft</t>
-  </si>
-  <si>
-    <t>34#435;'/.</t>
-  </si>
-  <si>
-    <t>8374GkJGF';</t>
-  </si>
-  <si>
-    <t>fttt</t>
-  </si>
-  <si>
-    <t>232@3746</t>
-  </si>
-  <si>
-    <t>sdjfh</t>
   </si>
   <si>
     <t>admin</t>
@@ -425,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -470,10 +455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,15 +477,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -511,71 +496,35 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>